<commit_message>
cambio en diseño y modelado
</commit_message>
<xml_diff>
--- a/datos/miembros.xlsx
+++ b/datos/miembros.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p1jav\OneDrive\Documents\GitHub\proyecto2_datos\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92544D48-7920-45E0-B680-5A021C86E114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E11E36-1761-4078-BACF-C56CD207740E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{51970689-DAAB-4DF8-9535-4814C8A418EA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{51970689-DAAB-4DF8-9535-4814C8A418EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="equipos" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -5579,15 +5580,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85F8894C-6C5D-4481-95C2-FFE44A18F8C7}">
   <dimension ref="A1:G736"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A532" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A556" sqref="A556"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G736" sqref="G1:G736"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -22522,4 +22523,3699 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5276D157-C07B-4EF5-B29F-420B566A9F6D}">
+  <dimension ref="A1:A736"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A736"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A133">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A134">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A135">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A136">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A137">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A138">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A139">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A140">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A141">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A142">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A143">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A144">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A145">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A146">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A147">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A148">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A149">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A150">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A151">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A152">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A153">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A154">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A155">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A156">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A157">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A158">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A159">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A160">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A161">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A162">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A163">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A164">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A165">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A166">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A167">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A168">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A169">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A170">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A171">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A172">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A173">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A174">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A175">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A176">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A177">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A178">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A179">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A180">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A181">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A182">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A183">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A184">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A185">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A186">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A187">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A188">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A189">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A190">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A191">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A192">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A193">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A194">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A195">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A196">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A197">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A198">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A199">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A200">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A201">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A202">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A203">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A204">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A205">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A206">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A207">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A208">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A209">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A210">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A211">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A212">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A213">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A214">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A215">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A216">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A217">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A218">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A219">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A220">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A221">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A222">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A223">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A224">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A225">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A226">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A227">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A228">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A229">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A230">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A231">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A232">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A233">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A234">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A235">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A236">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A237">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A238">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A239">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A240">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A241">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A242">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A243">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A244">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A245">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A246">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A247">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A248">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A249">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A250">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A251">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A252">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A253">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A254">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A255">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A256">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A257">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A258">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A259">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A260">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A261">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A262">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A263">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A264">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A265">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A266">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A267">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A268">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A269">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A270">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A271">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A272">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A273">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A274">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A275">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A276">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A277">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A278">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A279">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A280">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A281">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A282">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A283">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A284">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A285">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A286">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A287">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A288">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A289">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A290">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A291">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A292">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A293">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A294">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A295">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A296">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A297">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A298">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A299">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A300">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A301">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A302">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A303">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A304">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A305">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A306">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A307">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A308">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A309">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A310">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A311">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A312">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A313">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A314">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A315">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A316">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A317">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A318">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A319">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A320">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A321">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A322">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A323">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A324">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A325">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A326">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A327">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A328">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A329">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A330">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A331">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A332">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A333">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A334">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A335">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A336">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A337">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A338">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A339">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A340">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A341">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A342">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A343">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A344">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A345">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A346">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A347">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A348">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A349">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A350">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A351">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A352">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A353">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A354">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A355">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A356">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A357">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A358">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A359">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A360">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A361">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A362">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A363">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A364">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A365">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A366">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A367">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A368">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A369">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A370">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A371">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A372">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A373">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A374">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A375">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A376">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A377">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A378">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A379">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A380">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A381">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A382">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A383">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A384">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A385">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A386">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A387">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A388">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A389">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A390">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A391">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A392">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A393">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A394">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A395">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A396">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A397">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A398">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A399">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A400">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A401">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A402">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A403">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A404">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A405">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A406">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A407">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A408">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A409">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A410">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A411">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A412">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A413">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A414">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A415">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A416">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A417">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A418">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A419">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A420">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A421">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A422">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A423">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A424">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A425">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A426">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A427">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A428">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="429" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A429">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A430">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A431">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A432">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A433">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A434">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A435">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A436">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A437">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A438">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A439">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A440">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A441">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A442">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A443">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A444">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A445">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A446">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A447">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A448">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A449">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A450">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A451">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A452">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="453" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A453">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="454" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A454">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A455">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A456">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="457" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A457">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="458" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A458">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A459">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A460">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="461" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A461">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="462" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A462">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="463" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A463">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A464">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A465">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A466">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A467">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A468">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A469">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A470">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A471">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A472">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A473">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A474">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A475">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="476" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A476">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A477">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A478">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="479" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A479">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="480" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A480">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="481" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A481">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="482" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A482">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="483" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A483">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="484" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A484">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="485" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A485">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="486" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A486">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="487" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A487">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="488" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A488">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="489" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A489">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="490" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A490">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="491" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A491">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="492" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A492">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="493" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A493">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="494" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A494">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="495" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A495">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="496" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A496">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="497" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A497">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="498" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A498">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="499" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A499">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A500">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="501" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A501">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="502" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A502">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="503" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A503">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="504" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A504">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="505" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A505">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="506" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A506">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="507" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A507">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="508" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A508">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="509" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A509">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="510" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A510">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="511" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A511">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="512" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A512">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="513" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A513">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A514">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A515">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="516" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A516">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="517" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A517">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="518" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A518">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="519" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A519">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="520" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A520">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="521" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A521">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="522" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A522">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="523" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A523">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="524" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A524">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="525" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A525">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="526" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A526">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="527" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A527">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="528" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A528">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="529" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A529">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="530" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A530">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="531" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A531">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="532" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A532">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="533" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A533">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="534" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A534">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="535" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A535">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="536" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A536">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="537" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A537">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="538" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A538">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="539" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A539">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="540" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A540">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="541" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A541">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="542" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A542">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="543" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A543">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="544" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A544">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="545" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A545">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="546" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A546">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="547" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A547">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="548" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A548">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="549" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A549">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="550" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A550">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="551" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A551">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="552" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A552">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="553" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A553">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="554" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A554">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="555" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A555">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="556" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A556">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="557" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A557">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="558" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A558">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="559" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A559">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="560" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A560">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="561" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A561">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="562" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A562">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="563" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A563">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="564" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A564">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="565" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A565">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="566" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A566">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="567" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A567">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="568" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A568">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="569" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A569">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="570" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A570">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="571" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A571">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="572" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A572">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="573" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A573">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="574" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A574">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="575" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A575">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="576" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A576">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="577" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A577">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="578" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A578">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="579" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A579">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="580" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A580">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="581" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A581">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="582" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A582">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="583" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A583">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="584" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A584">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="585" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A585">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="586" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A586">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="587" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A587">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="588" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A588">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="589" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A589">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="590" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A590">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="591" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A591">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="592" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A592">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="593" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A593">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="594" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A594">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="595" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A595">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="596" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A596">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="597" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A597">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="598" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A598">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="599" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A599">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="600" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A600">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="601" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A601">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="602" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A602">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="603" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A603">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="604" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A604">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="605" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A605">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="606" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A606">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="607" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A607">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="608" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A608">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="609" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A609">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="610" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A610">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="611" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A611">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="612" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A612">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="613" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A613">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="614" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A614">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="615" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A615">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="616" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A616">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="617" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A617">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="618" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A618">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="619" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A619">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="620" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A620">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="621" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A621">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="622" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A622">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="623" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A623">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="624" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A624">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="625" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A625">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="626" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A626">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="627" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A627">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="628" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A628">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="629" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A629">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="630" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A630">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="631" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A631">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="632" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A632">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="633" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A633">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="634" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A634">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="635" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A635">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="636" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A636">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="637" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A637">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="638" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A638">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="639" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A639">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="640" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A640">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="641" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A641">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="642" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A642">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="643" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A643">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="644" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A644">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="645" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A645">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="646" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A646">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="647" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A647">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="648" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A648">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="649" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A649">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="650" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A650">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="651" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A651">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="652" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A652">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="653" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A653">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="654" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A654">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="655" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A655">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="656" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A656">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="657" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A657">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="658" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A658">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="659" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A659">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="660" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A660">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="661" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A661">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="662" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A662">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="663" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A663">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="664" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A664">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="665" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A665">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="666" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A666">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="667" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A667">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="668" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A668">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="669" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A669">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="670" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A670">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="671" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A671">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="672" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A672">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="673" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A673">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="674" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A674">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="675" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A675">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="676" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A676">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="677" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A677">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="678" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A678">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="679" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A679">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="680" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A680">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="681" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A681">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="682" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A682">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="683" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A683">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="684" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A684">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="685" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A685">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="686" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A686">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="687" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A687">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="688" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A688">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="689" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A689">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="690" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A690">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="691" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A691">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="692" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A692">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="693" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A693">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="694" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A694">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="695" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A695">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="696" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A696">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="697" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A697">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="698" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A698">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="699" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A699">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="700" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A700">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="701" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A701">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="702" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A702">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="703" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A703">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="704" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A704">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="705" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A705">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="706" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A706">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="707" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A707">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="708" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A708">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="709" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A709">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="710" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A710">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="711" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A711">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="712" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A712">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="713" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A713">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="714" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A714">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="715" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A715">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="716" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A716">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="717" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A717">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="718" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A718">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="719" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A719">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="720" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A720">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="721" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A721">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="722" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A722">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="723" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A723">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="724" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A724">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="725" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A725">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="726" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A726">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="727" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A727">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="728" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A728">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="729" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A729">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="730" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A730">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="731" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A731">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="732" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A732">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="733" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A733">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="734" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A734">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="735" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A735">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="736" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A736">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>